<commit_message>
update paramsASR for consistent label column notation
</commit_message>
<xml_diff>
--- a/inst/extdata/ParameterMapping.xlsx
+++ b/inst/extdata/ParameterMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d8cbaaa4eaa566d/Documents/1 ACASAK/MassWateR/Continuous data/Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\AquaSensR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D3A92422-55C1-40C4-AC6C-4A7F06D065B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEB6B13A-E07B-409E-87F0-A0256501415E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81CA37A-6788-4DB1-8233-944F8D061139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous Parameters" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <author>Benjamen Wetherill</author>
   </authors>
   <commentList>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{2A8F7830-A261-4C82-B8E0-3FB8F97F010D}">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{2A8F7830-A261-4C82-B8E0-3FB8F97F010D}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
   <si>
     <t>Water Temp</t>
   </si>
@@ -196,30 +196,6 @@
     <t>RFU</t>
   </si>
   <si>
-    <t>Air_Temp_C</t>
-  </si>
-  <si>
-    <t>Air_Temp_F</t>
-  </si>
-  <si>
-    <t>Water_Temp_C</t>
-  </si>
-  <si>
-    <t>Water_Temp_F</t>
-  </si>
-  <si>
-    <t>Air_BP_psi</t>
-  </si>
-  <si>
-    <t>Water_P_psi</t>
-  </si>
-  <si>
-    <t>Sensor_Depth_ft</t>
-  </si>
-  <si>
-    <t>Gage_Height_ft</t>
-  </si>
-  <si>
     <t>Salinity_ppt</t>
   </si>
   <si>
@@ -241,15 +217,9 @@
     <t>Conductivity_uS_cm</t>
   </si>
   <si>
-    <t>Sp_Conductance_uS_cm</t>
-  </si>
-  <si>
     <t>DO_mg_L</t>
   </si>
   <si>
-    <t>DO_adj_mg_L</t>
-  </si>
-  <si>
     <t>DO_pctsat</t>
   </si>
   <si>
@@ -278,6 +248,57 @@
   </si>
   <si>
     <t>#/100ml</t>
+  </si>
+  <si>
+    <t>Air Temp_C</t>
+  </si>
+  <si>
+    <t>Air Temp_F</t>
+  </si>
+  <si>
+    <t>Water Temp_C</t>
+  </si>
+  <si>
+    <t>Water Temp_F</t>
+  </si>
+  <si>
+    <t>Air BP_psi</t>
+  </si>
+  <si>
+    <t>Water P_psi</t>
+  </si>
+  <si>
+    <t>Sensor Depth_ft</t>
+  </si>
+  <si>
+    <t>Gage Height_ft</t>
+  </si>
+  <si>
+    <t>Sp Conductance_uS_cm</t>
+  </si>
+  <si>
+    <t>DO adj_mg_L</t>
+  </si>
+  <si>
+    <t>Salinity_psu</t>
+  </si>
+  <si>
+    <t>psu</t>
+  </si>
+  <si>
+    <t>Solids</t>
+  </si>
+  <si>
+    <t>Total dissolved solids</t>
+  </si>
+  <si>
+    <t>TDS_mg_L</t>
+  </si>
+  <si>
+    <t>TSS_mg_L</t>
+  </si>
+  <si>
+    <t>Total suspended solids</t>
   </si>
 </sst>
 </file>
@@ -662,24 +683,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BB29DB-B39A-4C45-B40C-840474EE5118}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="58.33203125" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -693,12 +714,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -707,12 +728,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -721,12 +742,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -735,12 +756,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -749,28 +770,28 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -779,12 +800,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -793,12 +814,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -807,12 +828,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -821,12 +842,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -835,12 +856,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -849,26 +870,26 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -877,190 +898,232 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>72</v>
+      <c r="D30" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Label column to paramsASR, update checkASRcont
</commit_message>
<xml_diff>
--- a/inst/extdata/ParameterMapping.xlsx
+++ b/inst/extdata/ParameterMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\AquaSensR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81CA37A-6788-4DB1-8233-944F8D061139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7D319B-89C7-4BA8-BF1B-39335FACBBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous Parameters" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
   <si>
     <t>Water Temp</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Phycocyanin (probe)</t>
   </si>
   <si>
-    <t>MassWateR Column Label</t>
-  </si>
-  <si>
     <t>WQX Unit of measure</t>
   </si>
   <si>
@@ -299,13 +296,127 @@
   </si>
   <si>
     <t>Total suspended solids</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Salinity (psu)</t>
+  </si>
+  <si>
+    <t>Turbidity (NTU)</t>
+  </si>
+  <si>
+    <t>Escherichia coli (#/100ml)</t>
+  </si>
+  <si>
+    <t>DO (mg/L)</t>
+  </si>
+  <si>
+    <t>DO (% Sat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH </t>
+  </si>
+  <si>
+    <t>Chlorophyll-a (RFU)</t>
+  </si>
+  <si>
+    <t>Pheophytin (RFU)</t>
+  </si>
+  <si>
+    <t>DO Adjusted (mg/L)</t>
+  </si>
+  <si>
+    <t>Air Temp (C)</t>
+  </si>
+  <si>
+    <t>Air Temp (F)</t>
+  </si>
+  <si>
+    <t>Water Temp (C)</t>
+  </si>
+  <si>
+    <t>Water Temp (F)</t>
+  </si>
+  <si>
+    <t>Barometric Pressure (PSI)</t>
+  </si>
+  <si>
+    <t>Water Level (PSI)</t>
+  </si>
+  <si>
+    <t>Sensor Depth (ft)</t>
+  </si>
+  <si>
+    <t>Gage Height (ft)</t>
+  </si>
+  <si>
+    <t>Discharge (cfs)</t>
+  </si>
+  <si>
+    <t>Salinity (ppt)</t>
+  </si>
+  <si>
+    <r>
+      <t>Conductivity (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>μ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S/cm)</t>
+    </r>
+  </si>
+  <si>
+    <t>Specific Conductance (μS/cm)</t>
+  </si>
+  <si>
+    <t>Pheophytin (μg/L)</t>
+  </si>
+  <si>
+    <t>Cyanobacteria (μg/L)</t>
+  </si>
+  <si>
+    <t>Phycocyanin (μg/L)</t>
+  </si>
+  <si>
+    <t>Phycoerythrin (μg/L)</t>
+  </si>
+  <si>
+    <t>Nitrate (μg/L)</t>
+  </si>
+  <si>
+    <t>Chlorophyll-a (μg/L)</t>
+  </si>
+  <si>
+    <t>Total Dissolved Solids (mg/L)</t>
+  </si>
+  <si>
+    <t>Total Suspended Solids (mg/L)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +430,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -683,447 +800,543 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BB29DB-B39A-4C45-B40C-840474EE5118}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="58.33203125" customWidth="1"/>
-    <col min="4" max="4" width="59.33203125" customWidth="1"/>
+    <col min="2" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" customWidth="1"/>
+    <col min="5" max="5" width="59.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="E31" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" t="s">
         <v>78</v>
       </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>39</v>
+      <c r="E32" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add workflow for metadata file
</commit_message>
<xml_diff>
--- a/inst/extdata/ParameterMapping.xlsx
+++ b/inst/extdata/ParameterMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\AquaSensR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7D319B-89C7-4BA8-BF1B-39335FACBBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8D484E-7359-47C4-9FCA-F18BA1278C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
@@ -438,30 +438,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -476,11 +458,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +782,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,16 +797,16 @@
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>80</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -838,16 +814,16 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>90</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -855,16 +831,16 @@
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>91</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -872,16 +848,16 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>92</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -889,16 +865,16 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>93</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -906,10 +882,10 @@
       <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>94</v>
       </c>
     </row>
@@ -917,10 +893,10 @@
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>95</v>
       </c>
     </row>
@@ -928,16 +904,16 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>96</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -945,16 +921,16 @@
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>97</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -962,16 +938,16 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>98</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -979,16 +955,16 @@
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>100</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -996,16 +972,16 @@
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>101</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1013,16 +989,16 @@
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>99</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1030,16 +1006,16 @@
       <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>81</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1047,16 +1023,16 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>84</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1064,16 +1040,16 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>89</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1081,16 +1057,16 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>85</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1098,16 +1074,16 @@
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>86</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1115,16 +1091,16 @@
       <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>82</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1132,16 +1108,16 @@
       <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>107</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1149,16 +1125,16 @@
       <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>87</v>
       </c>
       <c r="D21" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1166,16 +1142,16 @@
       <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>102</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1183,16 +1159,16 @@
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>88</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1200,16 +1176,16 @@
       <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>103</v>
       </c>
       <c r="D24" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1217,16 +1193,16 @@
       <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>104</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1234,16 +1210,16 @@
       <c r="A26" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>105</v>
       </c>
       <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1251,16 +1227,16 @@
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>106</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1268,40 +1244,38 @@
       <c r="A28" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" t="s">
         <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1309,16 +1283,16 @@
       <c r="A31" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>108</v>
       </c>
       <c r="D31" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1326,16 +1300,16 @@
       <c r="A32" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" t="s">
         <v>109</v>
       </c>
       <c r="D32" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>